<commit_message>
Atualização de planilha detalhada da Sprint.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Sprint-Backlog-Sprint-03# DETALHADO.xlsx
+++ b/Trunk/Doc/Sprint-Backlog-Sprint-03# DETALHADO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\Unibratec\Repositorios\fusioness\Trunk\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.dinarte\Documents\Unibratec\fusioness\Trunk\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="20490" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint-Backlog" sheetId="2" r:id="rId1"/>
@@ -293,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,7 +659,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -686,10 +692,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -710,9 +722,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -722,201 +731,216 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="185">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -935,7 +959,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1371,11 +1395,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1782257904"/>
-        <c:axId val="-1782259536"/>
+        <c:axId val="258601400"/>
+        <c:axId val="258602184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1782257904"/>
+        <c:axId val="258601400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1419,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1782259536"/>
+        <c:crossAx val="258602184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1403,7 +1427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1782259536"/>
+        <c:axId val="258602184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1454,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1782257904"/>
+        <c:crossAx val="258601400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1773,15 +1797,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="15" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="2" customWidth="1"/>
     <col min="6" max="19" width="4.7109375" style="2" customWidth="1"/>
@@ -1789,88 +1813,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="18"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1915,11 +1939,11 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="3">
         <f>SUM(F7:F9)+SUM(F11:F13)</f>
         <v>20</v>
@@ -1977,401 +2001,401 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:19" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
+      <c r="D6" s="27"/>
+      <c r="E6" s="27">
         <v>10</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9" t="s">
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+    </row>
+    <row r="7" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="9">
-        <v>8</v>
-      </c>
-      <c r="F7" s="9">
-        <v>8</v>
-      </c>
-      <c r="G7" s="9">
-        <v>8</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="E7" s="30">
+        <v>8</v>
+      </c>
+      <c r="F7" s="30">
+        <v>8</v>
+      </c>
+      <c r="G7" s="30">
+        <v>8</v>
+      </c>
+      <c r="H7" s="30">
         <v>7</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="30">
         <v>7</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="30">
         <v>7</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="30">
         <v>7</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="30">
         <v>7</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="30">
         <v>7</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="30">
         <v>7</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="30">
         <v>7</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="30">
         <v>7</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q7" s="30">
         <v>7</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R7" s="30">
         <v>7</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="30">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="10">
-        <v>1</v>
-      </c>
-      <c r="I8" s="10">
-        <v>1</v>
-      </c>
-      <c r="J8" s="10">
-        <v>1</v>
-      </c>
-      <c r="K8" s="10">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10">
-        <v>1</v>
-      </c>
-      <c r="M8" s="10">
-        <v>1</v>
-      </c>
-      <c r="N8" s="10">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10">
-        <v>1</v>
-      </c>
-      <c r="P8" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>1</v>
-      </c>
-      <c r="R8" s="10">
-        <v>1</v>
-      </c>
-      <c r="S8" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
+      <c r="E8" s="31">
+        <v>1</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1</v>
+      </c>
+      <c r="G8" s="31">
+        <v>1</v>
+      </c>
+      <c r="H8" s="31">
+        <v>1</v>
+      </c>
+      <c r="I8" s="31">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31">
+        <v>1</v>
+      </c>
+      <c r="K8" s="31">
+        <v>1</v>
+      </c>
+      <c r="L8" s="31">
+        <v>1</v>
+      </c>
+      <c r="M8" s="31">
+        <v>1</v>
+      </c>
+      <c r="N8" s="31">
+        <v>1</v>
+      </c>
+      <c r="O8" s="31">
+        <v>1</v>
+      </c>
+      <c r="P8" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="31">
+        <v>1</v>
+      </c>
+      <c r="R8" s="31">
+        <v>1</v>
+      </c>
+      <c r="S8" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="10">
-        <v>1</v>
-      </c>
-      <c r="I9" s="10">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10">
-        <v>1</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1</v>
-      </c>
-      <c r="L9" s="10">
-        <v>1</v>
-      </c>
-      <c r="M9" s="10">
-        <v>1</v>
-      </c>
-      <c r="N9" s="10">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10">
-        <v>1</v>
-      </c>
-      <c r="P9" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>1</v>
-      </c>
-      <c r="R9" s="10">
-        <v>1</v>
-      </c>
-      <c r="S9" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="E9" s="31">
+        <v>1</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1</v>
+      </c>
+      <c r="I9" s="31">
+        <v>1</v>
+      </c>
+      <c r="J9" s="31">
+        <v>1</v>
+      </c>
+      <c r="K9" s="31">
+        <v>1</v>
+      </c>
+      <c r="L9" s="31">
+        <v>1</v>
+      </c>
+      <c r="M9" s="31">
+        <v>1</v>
+      </c>
+      <c r="N9" s="31">
+        <v>1</v>
+      </c>
+      <c r="O9" s="31">
+        <v>1</v>
+      </c>
+      <c r="P9" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="31">
+        <v>1</v>
+      </c>
+      <c r="R9" s="31">
+        <v>1</v>
+      </c>
+      <c r="S9" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="29" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row r="11" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+    </row>
+    <row r="11" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="9">
-        <v>8</v>
-      </c>
-      <c r="F11" s="9">
-        <v>8</v>
-      </c>
-      <c r="G11" s="9">
-        <v>8</v>
-      </c>
-      <c r="H11" s="9">
-        <v>8</v>
-      </c>
-      <c r="I11" s="9">
-        <v>8</v>
-      </c>
-      <c r="J11" s="9">
-        <v>8</v>
-      </c>
-      <c r="K11" s="9">
-        <v>8</v>
-      </c>
-      <c r="L11" s="9">
-        <v>8</v>
-      </c>
-      <c r="M11" s="9">
-        <v>8</v>
-      </c>
-      <c r="N11" s="9">
-        <v>8</v>
-      </c>
-      <c r="O11" s="9">
-        <v>8</v>
-      </c>
-      <c r="P11" s="9">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>8</v>
-      </c>
-      <c r="R11" s="9">
-        <v>8</v>
-      </c>
-      <c r="S11" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10" t="s">
+      <c r="E11" s="30">
+        <v>8</v>
+      </c>
+      <c r="F11" s="30">
+        <v>8</v>
+      </c>
+      <c r="G11" s="30">
+        <v>8</v>
+      </c>
+      <c r="H11" s="30">
+        <v>8</v>
+      </c>
+      <c r="I11" s="30">
+        <v>8</v>
+      </c>
+      <c r="J11" s="30">
+        <v>8</v>
+      </c>
+      <c r="K11" s="30">
+        <v>8</v>
+      </c>
+      <c r="L11" s="30">
+        <v>8</v>
+      </c>
+      <c r="M11" s="30">
+        <v>8</v>
+      </c>
+      <c r="N11" s="30">
+        <v>8</v>
+      </c>
+      <c r="O11" s="30">
+        <v>8</v>
+      </c>
+      <c r="P11" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="30">
+        <v>8</v>
+      </c>
+      <c r="R11" s="30">
+        <v>8</v>
+      </c>
+      <c r="S11" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1</v>
-      </c>
-      <c r="I12" s="10">
-        <v>1</v>
-      </c>
-      <c r="J12" s="10">
-        <v>1</v>
-      </c>
-      <c r="K12" s="10">
-        <v>1</v>
-      </c>
-      <c r="L12" s="10">
-        <v>1</v>
-      </c>
-      <c r="M12" s="10">
-        <v>1</v>
-      </c>
-      <c r="N12" s="10">
-        <v>1</v>
-      </c>
-      <c r="O12" s="10">
-        <v>1</v>
-      </c>
-      <c r="P12" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="10">
-        <v>1</v>
-      </c>
-      <c r="R12" s="10">
-        <v>1</v>
-      </c>
-      <c r="S12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
+      <c r="E12" s="31">
+        <v>1</v>
+      </c>
+      <c r="F12" s="31">
+        <v>1</v>
+      </c>
+      <c r="G12" s="31">
+        <v>1</v>
+      </c>
+      <c r="H12" s="31">
+        <v>1</v>
+      </c>
+      <c r="I12" s="31">
+        <v>1</v>
+      </c>
+      <c r="J12" s="31">
+        <v>1</v>
+      </c>
+      <c r="K12" s="31">
+        <v>1</v>
+      </c>
+      <c r="L12" s="31">
+        <v>1</v>
+      </c>
+      <c r="M12" s="31">
+        <v>1</v>
+      </c>
+      <c r="N12" s="31">
+        <v>1</v>
+      </c>
+      <c r="O12" s="31">
+        <v>1</v>
+      </c>
+      <c r="P12" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="31">
+        <v>1</v>
+      </c>
+      <c r="R12" s="31">
+        <v>1</v>
+      </c>
+      <c r="S12" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="10">
-        <v>1</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
-      </c>
-      <c r="G13" s="10">
-        <v>1</v>
-      </c>
-      <c r="H13" s="10">
-        <v>1</v>
-      </c>
-      <c r="I13" s="10">
-        <v>1</v>
-      </c>
-      <c r="J13" s="10">
-        <v>1</v>
-      </c>
-      <c r="K13" s="10">
-        <v>1</v>
-      </c>
-      <c r="L13" s="10">
-        <v>1</v>
-      </c>
-      <c r="M13" s="10">
-        <v>1</v>
-      </c>
-      <c r="N13" s="10">
-        <v>1</v>
-      </c>
-      <c r="O13" s="10">
-        <v>1</v>
-      </c>
-      <c r="P13" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>1</v>
-      </c>
-      <c r="R13" s="10">
-        <v>1</v>
-      </c>
-      <c r="S13" s="10">
+      <c r="E13" s="31">
+        <v>1</v>
+      </c>
+      <c r="F13" s="31">
+        <v>1</v>
+      </c>
+      <c r="G13" s="31">
+        <v>1</v>
+      </c>
+      <c r="H13" s="31">
+        <v>1</v>
+      </c>
+      <c r="I13" s="31">
+        <v>1</v>
+      </c>
+      <c r="J13" s="31">
+        <v>1</v>
+      </c>
+      <c r="K13" s="31">
+        <v>1</v>
+      </c>
+      <c r="L13" s="31">
+        <v>1</v>
+      </c>
+      <c r="M13" s="31">
+        <v>1</v>
+      </c>
+      <c r="N13" s="31">
+        <v>1</v>
+      </c>
+      <c r="O13" s="31">
+        <v>1</v>
+      </c>
+      <c r="P13" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="31">
+        <v>1</v>
+      </c>
+      <c r="R13" s="31">
+        <v>1</v>
+      </c>
+      <c r="S13" s="31">
         <v>1</v>
       </c>
     </row>
@@ -2382,7 +2406,7 @@
       <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="4"/>
@@ -2409,7 +2433,7 @@
       <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -2466,7 +2490,7 @@
       <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -2523,7 +2547,7 @@
       <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -2582,7 +2606,7 @@
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="4"/>
@@ -2607,7 +2631,7 @@
       <c r="B19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -2664,7 +2688,7 @@
       <c r="B20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -2721,7 +2745,7 @@
       <c r="B21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -2780,7 +2804,7 @@
       <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D22" s="4"/>
@@ -2807,7 +2831,7 @@
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -2864,7 +2888,7 @@
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -2921,7 +2945,7 @@
       <c r="B25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -2980,7 +3004,7 @@
       <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="4"/>
@@ -3007,7 +3031,7 @@
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -3064,7 +3088,7 @@
       <c r="B28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -3121,7 +3145,7 @@
       <c r="B29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -3173,399 +3197,399 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="150" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+    <row r="30" spans="1:19" s="29" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A30" s="27">
         <v>41</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-    </row>
-    <row r="31" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9" t="s">
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+    </row>
+    <row r="31" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="9">
-        <v>8</v>
-      </c>
-      <c r="F31" s="9">
-        <v>8</v>
-      </c>
-      <c r="G31" s="9">
-        <v>8</v>
-      </c>
-      <c r="H31" s="9">
-        <v>8</v>
-      </c>
-      <c r="I31" s="9">
-        <v>8</v>
-      </c>
-      <c r="J31" s="9">
-        <v>8</v>
-      </c>
-      <c r="K31" s="9">
-        <v>8</v>
-      </c>
-      <c r="L31" s="9">
-        <v>8</v>
-      </c>
-      <c r="M31" s="9">
-        <v>8</v>
-      </c>
-      <c r="N31" s="9">
-        <v>8</v>
-      </c>
-      <c r="O31" s="9">
-        <v>8</v>
-      </c>
-      <c r="P31" s="9">
-        <v>8</v>
-      </c>
-      <c r="Q31" s="9">
-        <v>8</v>
-      </c>
-      <c r="R31" s="9">
-        <v>8</v>
-      </c>
-      <c r="S31" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10" t="s">
+      <c r="E31" s="30">
+        <v>8</v>
+      </c>
+      <c r="F31" s="30">
+        <v>8</v>
+      </c>
+      <c r="G31" s="30">
+        <v>8</v>
+      </c>
+      <c r="H31" s="30">
+        <v>8</v>
+      </c>
+      <c r="I31" s="30">
+        <v>8</v>
+      </c>
+      <c r="J31" s="30">
+        <v>8</v>
+      </c>
+      <c r="K31" s="30">
+        <v>8</v>
+      </c>
+      <c r="L31" s="30">
+        <v>8</v>
+      </c>
+      <c r="M31" s="30">
+        <v>8</v>
+      </c>
+      <c r="N31" s="30">
+        <v>8</v>
+      </c>
+      <c r="O31" s="30">
+        <v>8</v>
+      </c>
+      <c r="P31" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q31" s="30">
+        <v>8</v>
+      </c>
+      <c r="R31" s="30">
+        <v>8</v>
+      </c>
+      <c r="S31" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="B32" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10">
-        <v>1</v>
-      </c>
-      <c r="G32" s="10">
-        <v>1</v>
-      </c>
-      <c r="H32" s="10">
-        <v>1</v>
-      </c>
-      <c r="I32" s="10">
-        <v>1</v>
-      </c>
-      <c r="J32" s="10">
-        <v>1</v>
-      </c>
-      <c r="K32" s="10">
-        <v>1</v>
-      </c>
-      <c r="L32" s="10">
-        <v>1</v>
-      </c>
-      <c r="M32" s="10">
-        <v>1</v>
-      </c>
-      <c r="N32" s="10">
-        <v>1</v>
-      </c>
-      <c r="O32" s="10">
-        <v>1</v>
-      </c>
-      <c r="P32" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="10">
-        <v>1</v>
-      </c>
-      <c r="R32" s="10">
-        <v>1</v>
-      </c>
-      <c r="S32" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10" t="s">
+      <c r="E32" s="31">
+        <v>1</v>
+      </c>
+      <c r="F32" s="31">
+        <v>1</v>
+      </c>
+      <c r="G32" s="31">
+        <v>1</v>
+      </c>
+      <c r="H32" s="31">
+        <v>1</v>
+      </c>
+      <c r="I32" s="31">
+        <v>1</v>
+      </c>
+      <c r="J32" s="31">
+        <v>1</v>
+      </c>
+      <c r="K32" s="31">
+        <v>1</v>
+      </c>
+      <c r="L32" s="31">
+        <v>1</v>
+      </c>
+      <c r="M32" s="31">
+        <v>1</v>
+      </c>
+      <c r="N32" s="31">
+        <v>1</v>
+      </c>
+      <c r="O32" s="31">
+        <v>1</v>
+      </c>
+      <c r="P32" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="31">
+        <v>1</v>
+      </c>
+      <c r="R32" s="31">
+        <v>1</v>
+      </c>
+      <c r="S32" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="10">
-        <v>1</v>
-      </c>
-      <c r="F33" s="10">
-        <v>1</v>
-      </c>
-      <c r="G33" s="10">
-        <v>1</v>
-      </c>
-      <c r="H33" s="10">
-        <v>1</v>
-      </c>
-      <c r="I33" s="10">
-        <v>1</v>
-      </c>
-      <c r="J33" s="10">
-        <v>1</v>
-      </c>
-      <c r="K33" s="10">
-        <v>1</v>
-      </c>
-      <c r="L33" s="10">
-        <v>1</v>
-      </c>
-      <c r="M33" s="10">
-        <v>1</v>
-      </c>
-      <c r="N33" s="10">
-        <v>1</v>
-      </c>
-      <c r="O33" s="10">
-        <v>1</v>
-      </c>
-      <c r="P33" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="10">
-        <v>1</v>
-      </c>
-      <c r="R33" s="10">
-        <v>1</v>
-      </c>
-      <c r="S33" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="E33" s="31">
+        <v>1</v>
+      </c>
+      <c r="F33" s="31">
+        <v>1</v>
+      </c>
+      <c r="G33" s="31">
+        <v>1</v>
+      </c>
+      <c r="H33" s="31">
+        <v>1</v>
+      </c>
+      <c r="I33" s="31">
+        <v>1</v>
+      </c>
+      <c r="J33" s="31">
+        <v>1</v>
+      </c>
+      <c r="K33" s="31">
+        <v>1</v>
+      </c>
+      <c r="L33" s="31">
+        <v>1</v>
+      </c>
+      <c r="M33" s="31">
+        <v>1</v>
+      </c>
+      <c r="N33" s="31">
+        <v>1</v>
+      </c>
+      <c r="O33" s="31">
+        <v>1</v>
+      </c>
+      <c r="P33" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="31">
+        <v>1</v>
+      </c>
+      <c r="R33" s="31">
+        <v>1</v>
+      </c>
+      <c r="S33" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" s="29" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A34" s="27">
         <v>39</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-    </row>
-    <row r="35" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9" t="s">
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+      <c r="S34" s="27"/>
+    </row>
+    <row r="35" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="9">
-        <v>8</v>
-      </c>
-      <c r="F35" s="9">
-        <v>8</v>
-      </c>
-      <c r="G35" s="9">
-        <v>8</v>
-      </c>
-      <c r="H35" s="9">
-        <v>8</v>
-      </c>
-      <c r="I35" s="9">
-        <v>8</v>
-      </c>
-      <c r="J35" s="9">
-        <v>8</v>
-      </c>
-      <c r="K35" s="9">
-        <v>8</v>
-      </c>
-      <c r="L35" s="9">
-        <v>8</v>
-      </c>
-      <c r="M35" s="9">
-        <v>8</v>
-      </c>
-      <c r="N35" s="9">
-        <v>8</v>
-      </c>
-      <c r="O35" s="9">
-        <v>8</v>
-      </c>
-      <c r="P35" s="9">
-        <v>8</v>
-      </c>
-      <c r="Q35" s="9">
-        <v>8</v>
-      </c>
-      <c r="R35" s="9">
-        <v>8</v>
-      </c>
-      <c r="S35" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10" t="s">
+      <c r="E35" s="30">
+        <v>8</v>
+      </c>
+      <c r="F35" s="30">
+        <v>8</v>
+      </c>
+      <c r="G35" s="30">
+        <v>8</v>
+      </c>
+      <c r="H35" s="30">
+        <v>8</v>
+      </c>
+      <c r="I35" s="30">
+        <v>8</v>
+      </c>
+      <c r="J35" s="30">
+        <v>8</v>
+      </c>
+      <c r="K35" s="30">
+        <v>8</v>
+      </c>
+      <c r="L35" s="30">
+        <v>8</v>
+      </c>
+      <c r="M35" s="30">
+        <v>8</v>
+      </c>
+      <c r="N35" s="30">
+        <v>8</v>
+      </c>
+      <c r="O35" s="30">
+        <v>8</v>
+      </c>
+      <c r="P35" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q35" s="30">
+        <v>8</v>
+      </c>
+      <c r="R35" s="30">
+        <v>8</v>
+      </c>
+      <c r="S35" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="10">
-        <v>1</v>
-      </c>
-      <c r="F36" s="10">
-        <v>1</v>
-      </c>
-      <c r="G36" s="10">
-        <v>1</v>
-      </c>
-      <c r="H36" s="10">
-        <v>1</v>
-      </c>
-      <c r="I36" s="10">
-        <v>1</v>
-      </c>
-      <c r="J36" s="10">
-        <v>1</v>
-      </c>
-      <c r="K36" s="10">
-        <v>1</v>
-      </c>
-      <c r="L36" s="10">
-        <v>1</v>
-      </c>
-      <c r="M36" s="10">
-        <v>1</v>
-      </c>
-      <c r="N36" s="10">
-        <v>1</v>
-      </c>
-      <c r="O36" s="10">
-        <v>1</v>
-      </c>
-      <c r="P36" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="10">
-        <v>1</v>
-      </c>
-      <c r="R36" s="10">
-        <v>1</v>
-      </c>
-      <c r="S36" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10" t="s">
+      <c r="E36" s="31">
+        <v>1</v>
+      </c>
+      <c r="F36" s="31">
+        <v>1</v>
+      </c>
+      <c r="G36" s="31">
+        <v>1</v>
+      </c>
+      <c r="H36" s="31">
+        <v>1</v>
+      </c>
+      <c r="I36" s="31">
+        <v>1</v>
+      </c>
+      <c r="J36" s="31">
+        <v>1</v>
+      </c>
+      <c r="K36" s="31">
+        <v>1</v>
+      </c>
+      <c r="L36" s="31">
+        <v>1</v>
+      </c>
+      <c r="M36" s="31">
+        <v>1</v>
+      </c>
+      <c r="N36" s="31">
+        <v>1</v>
+      </c>
+      <c r="O36" s="31">
+        <v>1</v>
+      </c>
+      <c r="P36" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="31">
+        <v>1</v>
+      </c>
+      <c r="R36" s="31">
+        <v>1</v>
+      </c>
+      <c r="S36" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="10">
-        <v>1</v>
-      </c>
-      <c r="F37" s="10">
-        <v>1</v>
-      </c>
-      <c r="G37" s="10">
-        <v>1</v>
-      </c>
-      <c r="H37" s="10">
-        <v>1</v>
-      </c>
-      <c r="I37" s="10">
-        <v>1</v>
-      </c>
-      <c r="J37" s="10">
-        <v>1</v>
-      </c>
-      <c r="K37" s="10">
-        <v>1</v>
-      </c>
-      <c r="L37" s="10">
-        <v>1</v>
-      </c>
-      <c r="M37" s="10">
-        <v>1</v>
-      </c>
-      <c r="N37" s="10">
-        <v>1</v>
-      </c>
-      <c r="O37" s="10">
-        <v>1</v>
-      </c>
-      <c r="P37" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="10">
-        <v>1</v>
-      </c>
-      <c r="R37" s="10">
-        <v>1</v>
-      </c>
-      <c r="S37" s="10">
+      <c r="E37" s="31">
+        <v>1</v>
+      </c>
+      <c r="F37" s="31">
+        <v>1</v>
+      </c>
+      <c r="G37" s="31">
+        <v>1</v>
+      </c>
+      <c r="H37" s="31">
+        <v>1</v>
+      </c>
+      <c r="I37" s="31">
+        <v>1</v>
+      </c>
+      <c r="J37" s="31">
+        <v>1</v>
+      </c>
+      <c r="K37" s="31">
+        <v>1</v>
+      </c>
+      <c r="L37" s="31">
+        <v>1</v>
+      </c>
+      <c r="M37" s="31">
+        <v>1</v>
+      </c>
+      <c r="N37" s="31">
+        <v>1</v>
+      </c>
+      <c r="O37" s="31">
+        <v>1</v>
+      </c>
+      <c r="P37" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="31">
+        <v>1</v>
+      </c>
+      <c r="R37" s="31">
+        <v>1</v>
+      </c>
+      <c r="S37" s="31">
         <v>1</v>
       </c>
     </row>
@@ -3576,7 +3600,7 @@
       <c r="B38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D38" s="4"/>
@@ -3603,7 +3627,7 @@
       <c r="B39" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="9" t="s">
@@ -3660,7 +3684,7 @@
       <c r="B40" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -3717,7 +3741,7 @@
       <c r="B41" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D41" s="9" t="s">
@@ -3776,7 +3800,7 @@
       <c r="B42" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D42" s="4"/>
@@ -3803,7 +3827,7 @@
       <c r="B43" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="9" t="s">
@@ -3860,7 +3884,7 @@
       <c r="B44" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -3917,7 +3941,7 @@
       <c r="B45" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D45" s="9" t="s">
@@ -3976,7 +4000,7 @@
       <c r="B46" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="12" t="s">
         <v>61</v>
       </c>
       <c r="D46" s="4"/>
@@ -4003,7 +4027,7 @@
       <c r="B47" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D47" s="9" t="s">
@@ -4060,7 +4084,7 @@
       <c r="B48" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="9" t="s">
@@ -4117,7 +4141,7 @@
       <c r="B49" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -4176,7 +4200,7 @@
       <c r="B50" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="12" t="s">
         <v>62</v>
       </c>
       <c r="D50" s="4"/>
@@ -4203,7 +4227,7 @@
       <c r="B51" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -4260,7 +4284,7 @@
       <c r="B52" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -4317,7 +4341,7 @@
       <c r="B53" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C53" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D53" s="9" t="s">
@@ -4376,7 +4400,7 @@
       <c r="B54" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D54" s="4"/>
@@ -4403,7 +4427,7 @@
       <c r="B55" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D55" s="9" t="s">
@@ -4460,7 +4484,7 @@
       <c r="B56" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -4517,7 +4541,7 @@
       <c r="B57" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="C57" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D57" s="9" t="s">
@@ -4576,7 +4600,7 @@
       <c r="B58" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D58" s="4"/>
@@ -4603,7 +4627,7 @@
       <c r="B59" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -4660,7 +4684,7 @@
       <c r="B60" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D60" s="9" t="s">
@@ -4717,7 +4741,7 @@
       <c r="B61" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="25" t="s">
+      <c r="C61" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D61" s="9" t="s">
@@ -4776,7 +4800,7 @@
       <c r="B62" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D62" s="4"/>
@@ -4803,7 +4827,7 @@
       <c r="B63" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D63" s="9" t="s">
@@ -4860,7 +4884,7 @@
       <c r="B64" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D64" s="9" t="s">
@@ -4917,7 +4941,7 @@
       <c r="B65" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D65" s="9" t="s">
@@ -4976,7 +5000,7 @@
       <c r="B66" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="12" t="s">
         <v>66</v>
       </c>
       <c r="D66" s="4"/>
@@ -5003,7 +5027,7 @@
       <c r="B67" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D67" s="9" t="s">
@@ -5060,7 +5084,7 @@
       <c r="B68" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -5117,7 +5141,7 @@
       <c r="B69" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -5176,7 +5200,7 @@
       <c r="B70" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D70" s="4"/>
@@ -5203,7 +5227,7 @@
       <c r="B71" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D71" s="9" t="s">
@@ -5260,7 +5284,7 @@
       <c r="B72" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C72" s="25" t="s">
+      <c r="C72" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -5317,7 +5341,7 @@
       <c r="B73" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="25" t="s">
+      <c r="C73" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D73" s="9" t="s">
@@ -5376,7 +5400,7 @@
       <c r="B74" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D74" s="4"/>
@@ -5403,7 +5427,7 @@
       <c r="B75" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D75" s="9" t="s">
@@ -5460,7 +5484,7 @@
       <c r="B76" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C76" s="25" t="s">
+      <c r="C76" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D76" s="9" t="s">
@@ -5517,7 +5541,7 @@
       <c r="B77" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C77" s="25" t="s">
+      <c r="C77" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D77" s="9" t="s">
@@ -5576,7 +5600,7 @@
       <c r="B78" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="12" t="s">
         <v>68</v>
       </c>
       <c r="D78" s="4"/>
@@ -5603,7 +5627,7 @@
       <c r="B79" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D79" s="9" t="s">
@@ -5660,7 +5684,7 @@
       <c r="B80" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="25" t="s">
+      <c r="C80" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D80" s="9" t="s">
@@ -5717,7 +5741,7 @@
       <c r="B81" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C81" s="25" t="s">
+      <c r="C81" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D81" s="9" t="s">
@@ -5776,7 +5800,7 @@
       <c r="B82" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="12" t="s">
         <v>69</v>
       </c>
       <c r="D82" s="4"/>
@@ -5803,7 +5827,7 @@
       <c r="B83" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D83" s="9" t="s">
@@ -5860,7 +5884,7 @@
       <c r="B84" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C84" s="25" t="s">
+      <c r="C84" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -5917,7 +5941,7 @@
       <c r="B85" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C85" s="25" t="s">
+      <c r="C85" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D85" s="9" t="s">
@@ -5976,7 +6000,7 @@
       <c r="B86" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C86" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D86" s="4"/>
@@ -6003,7 +6027,7 @@
       <c r="B87" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D87" s="9" t="s">
@@ -6060,7 +6084,7 @@
       <c r="B88" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C88" s="25" t="s">
+      <c r="C88" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -6117,7 +6141,7 @@
       <c r="B89" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C89" s="25" t="s">
+      <c r="C89" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D89" s="9" t="s">
@@ -6176,7 +6200,7 @@
       <c r="B90" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D90" s="4"/>
@@ -6203,7 +6227,7 @@
       <c r="B91" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C91" s="24" t="s">
+      <c r="C91" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D91" s="9" t="s">
@@ -6260,7 +6284,7 @@
       <c r="B92" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C92" s="25" t="s">
+      <c r="C92" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -6317,7 +6341,7 @@
       <c r="B93" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C93" s="25" t="s">
+      <c r="C93" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D93" s="9" t="s">
@@ -6376,7 +6400,7 @@
       <c r="B94" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D94" s="4"/>
@@ -6403,7 +6427,7 @@
       <c r="B95" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C95" s="24" t="s">
+      <c r="C95" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D95" s="9" t="s">
@@ -6460,7 +6484,7 @@
       <c r="B96" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C96" s="25" t="s">
+      <c r="C96" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D96" s="9" t="s">
@@ -6517,7 +6541,7 @@
       <c r="B97" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C97" s="25" t="s">
+      <c r="C97" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D97" s="9" t="s">
@@ -6576,7 +6600,7 @@
       <c r="B98" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D98" s="4"/>
@@ -6603,7 +6627,7 @@
       <c r="B99" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C99" s="20" t="s">
+      <c r="C99" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D99" s="9" t="s">
@@ -6660,7 +6684,7 @@
       <c r="B100" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C100" s="20" t="s">
+      <c r="C100" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D100" s="9" t="s">
@@ -6717,7 +6741,7 @@
       <c r="B101" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C101" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D101" s="9" t="s">
@@ -6776,7 +6800,7 @@
       <c r="B102" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C102" s="20" t="s">
+      <c r="C102" s="12" t="s">
         <v>74</v>
       </c>
       <c r="D102" s="4"/>
@@ -6803,7 +6827,7 @@
       <c r="B103" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C103" s="24" t="s">
+      <c r="C103" s="13" t="s">
         <v>56</v>
       </c>
       <c r="D103" s="9" t="s">
@@ -6860,7 +6884,7 @@
       <c r="B104" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C104" s="25" t="s">
+      <c r="C104" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D104" s="9" t="s">
@@ -6917,7 +6941,7 @@
       <c r="B105" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C105" s="25" t="s">
+      <c r="C105" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D105" s="9" t="s">
@@ -6971,14 +6995,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:S2"/>
     <mergeCell ref="F3:S3"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:S2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>